<commit_message>
Added official name to migration huts
</commit_message>
<xml_diff>
--- a/storage/importer/huts/EUMA_HUTS_FPSM.xlsx
+++ b/storage/importer/huts/EUMA_HUTS_FPSM.xlsx
@@ -11,7 +11,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mizjMw8xETwuyL/3ykZmP0RiNzejg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miB/ihkVvMRwLdHpw/2TMd3T8KYRw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +31,7 @@
 Shelter</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L11">
+    <comment authorId="0" ref="M11">
       <text>
         <t xml:space="preserve">======
 ID#AAAALdFT2yo
@@ -39,7 +39,7 @@
 Formally owned by the Municipality, but based on а contract it is granted for use to the Mountain Club Lisec</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L7">
+    <comment authorId="0" ref="M7">
       <text>
         <t xml:space="preserve">======
 ID#AAAALdFT2yg
@@ -47,7 +47,7 @@
 А lawsuit is currently pending to return the building to the Mounteneering Federation.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L8">
+    <comment authorId="0" ref="M8">
       <text>
         <t xml:space="preserve">======
 ID#AAAALdFT2yc
@@ -55,7 +55,7 @@
 Formally owned by the Government, but by а decision of the Government ит is granted for permanent use to the Mounteneering Federation</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2">
+    <comment authorId="0" ref="M2">
       <text>
         <t xml:space="preserve">======
 ID#AAAALdFT2yQ
@@ -63,7 +63,7 @@
 The mountain hut is owned by the private construction company "Beton", but based on a contrac is operated by the MC Transverzalec.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L9">
+    <comment authorId="0" ref="M9">
       <text>
         <t xml:space="preserve">======
 ID#AAAALdFT2yM
@@ -82,14 +82,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgklvgEltZjbVqm6XQr+B3AJmnxGg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgWP5abZR+Em56R+FKrHjalyrqQmw=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="130">
   <si>
     <t>general questions</t>
   </si>
@@ -106,7 +106,10 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
+    <t>official_name</t>
+  </si>
+  <si>
+    <t>second_official_name</t>
   </si>
   <si>
     <t>description</t>
@@ -640,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -657,6 +660,9 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -2151,28 +2157,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="46.57"/>
-    <col customWidth="1" min="4" max="4" width="12.0"/>
-    <col customWidth="1" min="5" max="5" width="12.14"/>
-    <col customWidth="1" min="6" max="6" width="11.71"/>
-    <col customWidth="1" min="7" max="7" width="9.14"/>
-    <col customWidth="1" min="8" max="8" width="15.14"/>
-    <col customWidth="1" min="9" max="9" width="81.86"/>
-    <col customWidth="1" min="10" max="11" width="24.14"/>
-    <col customWidth="1" min="12" max="12" width="20.14"/>
-    <col customWidth="1" min="13" max="13" width="28.86"/>
-    <col customWidth="1" min="14" max="14" width="8.14"/>
+    <col customWidth="1" min="2" max="3" width="18.14"/>
+    <col customWidth="1" min="4" max="4" width="46.57"/>
+    <col customWidth="1" min="5" max="5" width="12.0"/>
+    <col customWidth="1" min="6" max="6" width="12.14"/>
+    <col customWidth="1" min="7" max="7" width="11.71"/>
+    <col customWidth="1" min="8" max="8" width="9.14"/>
+    <col customWidth="1" min="9" max="9" width="15.14"/>
+    <col customWidth="1" min="10" max="10" width="81.86"/>
+    <col customWidth="1" min="11" max="12" width="24.14"/>
+    <col customWidth="1" min="13" max="13" width="20.14"/>
+    <col customWidth="1" min="14" max="14" width="28.86"/>
+    <col customWidth="1" min="15" max="15" width="8.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -2190,13 +2196,13 @@
       <c r="H1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="11" t="s">
@@ -2205,40 +2211,41 @@
       <c r="M1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="13"/>
+      <c r="N1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" ht="27.0" customHeight="1">
-      <c r="A2" s="14">
+      <c r="A2" s="15">
         <v>1.0</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="16">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="17">
         <v>42.0158333</v>
       </c>
-      <c r="E2" s="16">
+      <c r="F2" s="17">
         <v>20.8777777</v>
       </c>
-      <c r="F2" s="17">
+      <c r="G2" s="18">
         <v>1800.0</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>19</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="21" t="s">
         <v>23</v>
       </c>
       <c r="L2" s="21" t="s">
@@ -2247,510 +2254,525 @@
       <c r="M2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="23"/>
+      <c r="N2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" ht="30.0" customHeight="1">
-      <c r="A3" s="14">
+      <c r="A3" s="15">
         <v>2.0</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="16">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="17">
         <v>41.0026621</v>
       </c>
-      <c r="E3" s="16">
+      <c r="F3" s="17">
         <v>21.1831915</v>
       </c>
-      <c r="F3" s="17">
+      <c r="G3" s="18">
         <v>2218.0</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="25" t="s">
         <v>29</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="26" t="s">
         <v>32</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="23"/>
+        <v>33</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" ht="21.0" customHeight="1">
-      <c r="A4" s="14">
+      <c r="A4" s="15">
         <v>3.0</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="16">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="17">
         <v>41.3561111</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F4" s="17">
         <v>22.8827777</v>
       </c>
-      <c r="F4" s="17">
+      <c r="G4" s="18">
         <v>1276.0</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="H4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>39</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="23"/>
+        <v>40</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="24"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="14">
+      <c r="A5" s="15">
         <v>4.0</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="16">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="17">
         <v>42.1844444</v>
       </c>
-      <c r="E5" s="16">
+      <c r="F5" s="17">
         <v>21.1244444</v>
       </c>
-      <c r="F5" s="17">
+      <c r="G5" s="18">
         <v>1625.0</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="H5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="23"/>
+      <c r="M5" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="14">
+      <c r="A6" s="15">
         <v>5.0</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="B6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17">
         <v>42.0163889</v>
       </c>
-      <c r="E6" s="16">
+      <c r="F6" s="17">
         <v>20.8766666</v>
       </c>
-      <c r="F6" s="17">
+      <c r="G6" s="18">
         <v>1820.0</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>48</v>
-      </c>
       <c r="H6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="19" t="s">
+      <c r="I6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="21" t="s">
-        <v>50</v>
+      <c r="L6" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="23"/>
+        <v>51</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="24"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>6.0</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="16">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="17">
         <v>7536119.34</v>
       </c>
-      <c r="E7" s="16">
+      <c r="F7" s="17">
         <v>4613425.54</v>
       </c>
-      <c r="F7" s="17">
+      <c r="G7" s="18">
         <v>1450.0</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="H7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="I7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>57</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="24"/>
     </row>
     <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="14">
+      <c r="A8" s="15">
         <v>7.0</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="16">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="17">
         <v>41.75</v>
       </c>
-      <c r="E8" s="16">
+      <c r="F8" s="17">
         <v>21.3333333</v>
       </c>
-      <c r="F8" s="17">
+      <c r="G8" s="18">
         <v>1450.0</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="H8" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="I8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="26" t="s">
         <v>64</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="23"/>
+        <v>65</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="24"/>
     </row>
     <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="14">
+      <c r="A9" s="15">
         <v>8.0</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="B9" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="17">
         <v>41.6416667</v>
       </c>
-      <c r="E9" s="16">
+      <c r="F9" s="17">
         <v>21.4386111</v>
       </c>
-      <c r="F9" s="17">
+      <c r="G9" s="18">
         <v>998.0</v>
       </c>
-      <c r="G9" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="I9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="25" t="s">
+      <c r="K9" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="26" t="s">
         <v>70</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="14">
+      <c r="A10" s="15">
         <v>9.0</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="16">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="17">
         <v>41.7422222</v>
       </c>
-      <c r="E10" s="14">
+      <c r="F10" s="15">
         <v>22.5011111</v>
       </c>
-      <c r="F10" s="17">
+      <c r="G10" s="18">
         <v>1420.0</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="26" t="s">
+      <c r="H10" s="31"/>
+      <c r="I10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="26" t="s">
         <v>76</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="23"/>
+        <v>77</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="14">
+      <c r="A11" s="15">
         <v>10.0</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="14">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="15">
         <v>41.7591667</v>
       </c>
-      <c r="E11" s="14">
+      <c r="F11" s="15">
         <v>22.4169444</v>
       </c>
-      <c r="F11" s="17">
+      <c r="G11" s="18">
         <v>1106.0</v>
       </c>
-      <c r="G11" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="19" t="s">
+      <c r="H11" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="19" t="s">
+      <c r="I11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="L11" s="21" t="s">
-        <v>70</v>
+      <c r="K11" s="32"/>
+      <c r="L11" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="14">
+      <c r="A12" s="15">
         <v>11.0</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="14">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="15">
         <v>42.0833333</v>
       </c>
-      <c r="E12" s="32">
+      <c r="F12" s="33">
         <v>20.8333333</v>
       </c>
-      <c r="F12" s="17">
+      <c r="G12" s="18">
         <v>2747.0</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="J12" s="26" t="s">
+      <c r="H12" s="31"/>
+      <c r="I12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="29" t="s">
         <v>87</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" ht="18.0" customHeight="1">
-      <c r="A13" s="14">
+      <c r="A13" s="15">
         <v>12.0</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="30">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="31">
         <v>42.1547222</v>
       </c>
-      <c r="E13" s="30">
+      <c r="F13" s="31">
         <v>21.4613888</v>
       </c>
-      <c r="F13" s="17">
+      <c r="G13" s="18">
         <v>1480.0</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="26" t="s">
+      <c r="H13" s="34"/>
+      <c r="I13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="29" t="s">
         <v>93</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" s="23"/>
+        <v>94</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="24"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="14">
+      <c r="A14" s="15">
         <v>13.0</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="14">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="15">
         <v>41.9871768</v>
       </c>
-      <c r="E14" s="14">
+      <c r="F14" s="15">
         <v>21.4173209</v>
       </c>
-      <c r="F14" s="17">
+      <c r="G14" s="18">
         <v>1060.0</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="28" t="s">
+      <c r="H14" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="I14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="L14" s="21" t="s">
-        <v>87</v>
+      <c r="L14" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="24"/>
     </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.15748031496062992" footer="0.0" header="0.0" left="0.75" right="0.11811023622047245" top="1.5208333333333333"/>
   <pageSetup paperSize="8" orientation="landscape"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="11" man="1"/>
+    <brk id="12" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -2786,116 +2808,116 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="C2" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="E2" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="G2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="I2" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="M2" s="35" t="s">
         <v>106</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="C3" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="G3" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="I3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="K3" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="M3" s="35" t="s">
         <v>113</v>
+      </c>
+      <c r="O3" s="35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="C4" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="34" t="s">
+      <c r="C4" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="E4" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="G4" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="I4" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="34" t="s">
+      <c r="K4" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="M4" s="35" t="s">
         <v>120</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="E5" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="34" t="s">
+      <c r="E5" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="I5" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="34" t="s">
+      <c r="K5" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="M5" s="35" t="s">
         <v>125</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="E6" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" s="34" t="s">
+      <c r="E6" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="O6" s="34" t="s">
-        <v>126</v>
+      <c r="I6" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="K7" s="34" t="s">
-        <v>128</v>
+      <c r="K7" s="35" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="K8" s="34" t="s">
-        <v>126</v>
+      <c r="K8" s="35" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1"/>

</xml_diff>